<commit_message>
Atualização automática de RONDA_ALTA.xlsx
</commit_message>
<xml_diff>
--- a/RONDA_ALTA.xlsx
+++ b/RONDA_ALTA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64B863B9-0A59-49D6-932F-FB686AC37DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9B11E9-499B-4232-92D8-20CF1133F681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1207,7 +1207,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{10188DF3-D3DB-4616-8A4A-9CEDCE620EFC}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{2479716D-7DB3-46DD-A271-50A95F0A9CC0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1237,10 +1237,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F05C75F-3A6A-466A-B14F-6A2A9687D43A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EE89982-6CA1-42CD-B78C-D695A3332E79}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1278,7 +1278,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2298E9C6-E2DB-47C9-BD2D-BB7BFC729379}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFAF7D31-21F0-41E1-8BDA-0C8E0AF5ACCF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1341,7 +1341,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E14D8382-4568-48DC-A7A9-5F04A71181B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55FEFD68-C1EB-4FFB-8C1F-797883244C87}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1360,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFC3F6A-205D-008B-35DF-7270B3DC99C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48A1495E-03D7-9CA4-F878-7EC4AEF0D3B8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1409,7 +1409,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D155F81-831E-BF8F-D592-24605BCB22D8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7687903-F307-8E4A-3B72-2D873A90A3AF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1428,7 +1428,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2778C77-DCCD-0DD2-13C7-4FE309F1D858}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FEE5A3E-2287-6C38-16BB-17F460520680}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1459,7 +1459,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41B6D003-6F54-C298-44BD-DA8D304F13D5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FF1D54C-9FF0-8886-3B99-DA9F05F21A15}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B4C5074-CC4B-C974-2193-44606CAA5AE7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB5B96C5-555B-6165-E2AB-73B58AEB3006}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1533,7 +1533,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{080D1914-B2F9-4843-87CF-2C2BF082F407}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CBDF991-7533-42A8-A03E-ECF77BAD7921}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E522D95-D092-46EA-8C84-54C9BE948C38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB108D6F-89B0-46D8-A9ED-C20994068EC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1614,7 +1614,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4AA0223-DC97-477F-9217-77592C5BF0CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34D7A011-D3A9-496D-9A1D-B5A55DED75C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1927,7 +1927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B92660-8B16-473E-9456-FD1200F28B56}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60132793-5BFF-44AF-A823-D59A7E3F628E}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>